<commit_message>
made changes in the baseclass and utility class
</commit_message>
<xml_diff>
--- a/TestScriptData/TestScriptData.xlsx
+++ b/TestScriptData/TestScriptData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{6507C689-9791-4469-AB40-532B330DAAF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{9566021D-49BE-431A-8A2D-53C6CC123BFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" activeTab="1" xr2:uid="{C23E2104-0086-4665-A45B-54629BE3B250}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{C23E2104-0086-4665-A45B-54629BE3B250}"/>
   </bookViews>
   <sheets>
     <sheet name="Org" sheetId="1" r:id="rId1"/>
@@ -13,7 +13,7 @@
     <sheet name="Product" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
+  <oleSize ref="A1:F15"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="54">
   <si>
     <t>TD_ID</t>
   </si>
@@ -616,8 +616,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E77A91DB-9B00-42FD-A8C1-282A0458EB4E}">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -818,8 +818,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE80524D-A10B-42B7-9406-E9205CB911A9}">
   <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -958,9 +958,7 @@
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="C10" s="3" t="s">
-        <v>53</v>
-      </c>
+      <c r="C10" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>